<commit_message>
missing chair + co-chair for last session fixed
</commit_message>
<xml_diff>
--- a/themes/Final Program 20190926.xlsx
+++ b/themes/Final Program 20190926.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emi/Dropbox (Personal)/Website/ysc2019/themes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philip\Dropbox\YSC2019\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3FF765-2543-834F-BF10-F9FFED74531B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCDEF07-3243-4085-940E-84E136EF7115}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="117">
   <si>
     <t>Day 1: Tuesday 1st October 2019</t>
   </si>
@@ -476,6 +476,21 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Computer science
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Chair: John Yeung
+Co-chair: Emi Tanaka</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="12"/>
@@ -523,17 +538,18 @@
     <t>Experiments on canola emergence for Ag Science students: project-based teaching of statistics</t>
   </si>
   <si>
-    <t>Margarita Moreno-Betancur Senior Research Fellow, VicBiostats</t>
-  </si>
-  <si>
     <t>Causal mediation analysis: bridging the gap with empirical science</t>
+  </si>
+  <si>
+    <t>Margarita Moreno-Betancur
+Senior Research Fellow, VicBiostats</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -559,6 +575,12 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -597,7 +619,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -657,6 +679,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -991,31 +1019,31 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="32.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="69.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="32.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1033,7 +1061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>0.375</v>
       </c>
@@ -1048,7 +1076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <f>A3+TIME(0,F3,0)</f>
         <v>0.37847222222222221</v>
@@ -1064,7 +1092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <f t="shared" ref="A5:A10" si="1">A4+TIME(0,F4,0)</f>
         <v>0.38541666666666663</v>
@@ -1077,16 +1105,16 @@
         <v>96</v>
       </c>
       <c r="D5" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="F5" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <f t="shared" si="1"/>
         <v>0.41666666666666663</v>
@@ -1095,8 +1123,8 @@
         <f t="shared" si="2"/>
         <v>0.42499999999999999</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>105</v>
+      <c r="C6" s="23" t="s">
+        <v>106</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>8</v>
@@ -1108,7 +1136,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <f t="shared" si="1"/>
         <v>0.42499999999999999</v>
@@ -1117,7 +1145,7 @@
         <f t="shared" si="2"/>
         <v>0.43333333333333335</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="10" t="s">
         <v>10</v>
       </c>
@@ -1128,7 +1156,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <f t="shared" si="1"/>
         <v>0.43333333333333335</v>
@@ -1137,7 +1165,7 @@
         <f t="shared" si="2"/>
         <v>0.44166666666666671</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="10" t="s">
         <v>12</v>
       </c>
@@ -1148,7 +1176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <f t="shared" si="1"/>
         <v>0.44166666666666671</v>
@@ -1157,7 +1185,7 @@
         <f t="shared" si="2"/>
         <v>0.45000000000000007</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="10" t="s">
         <v>89</v>
       </c>
@@ -1168,7 +1196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <f t="shared" si="1"/>
         <v>0.45000000000000007</v>
@@ -1177,7 +1205,7 @@
         <f t="shared" si="2"/>
         <v>0.45833333333333343</v>
       </c>
-      <c r="C10" s="21"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="18" t="s">
         <v>23</v>
       </c>
@@ -1188,7 +1216,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f>A10+TIME(0,F10,0)</f>
         <v>0.45833333333333343</v>
@@ -1206,7 +1234,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <f t="shared" ref="A12:A18" si="4">A11+TIME(0,F11,0)</f>
         <v>0.47916666666666674</v>
@@ -1215,7 +1243,7 @@
         <f t="shared" si="3"/>
         <v>0.4875000000000001</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="23" t="s">
         <v>101</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -1228,7 +1256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <f t="shared" si="4"/>
         <v>0.4875000000000001</v>
@@ -1237,7 +1265,7 @@
         <f t="shared" si="3"/>
         <v>0.49583333333333346</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="9" t="s">
         <v>17</v>
       </c>
@@ -1248,7 +1276,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <f t="shared" si="4"/>
         <v>0.49583333333333346</v>
@@ -1257,7 +1285,7 @@
         <f t="shared" si="3"/>
         <v>0.50416666666666676</v>
       </c>
-      <c r="C14" s="21"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="9" t="s">
         <v>19</v>
       </c>
@@ -1268,7 +1296,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <f t="shared" si="4"/>
         <v>0.50416666666666676</v>
@@ -1277,7 +1305,7 @@
         <f t="shared" si="3"/>
         <v>0.51250000000000007</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="9" t="s">
         <v>21</v>
       </c>
@@ -1288,7 +1316,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <f t="shared" si="4"/>
         <v>0.51250000000000007</v>
@@ -1297,7 +1325,7 @@
         <f t="shared" si="3"/>
         <v>0.52083333333333337</v>
       </c>
-      <c r="C16" s="21"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="18" t="s">
         <v>25</v>
       </c>
@@ -1308,7 +1336,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <f t="shared" si="4"/>
         <v>0.52083333333333337</v>
@@ -1317,7 +1345,7 @@
         <f t="shared" si="3"/>
         <v>0.52777777777777779</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="18" t="s">
         <v>27</v>
       </c>
@@ -1328,7 +1356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <f t="shared" si="4"/>
         <v>0.52777777777777779</v>
@@ -1337,18 +1365,18 @@
         <f t="shared" si="3"/>
         <v>0.53125</v>
       </c>
-      <c r="C18" s="21"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F18" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f>A18+TIME(0,F18,0)</f>
         <v>0.53125</v>
@@ -1366,7 +1394,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <f t="shared" ref="A20" si="6">A19+TIME(0,F19,0)</f>
         <v>0.57291666666666663</v>
@@ -1379,16 +1407,16 @@
         <v>97</v>
       </c>
       <c r="D20" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="F20" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <f t="shared" ref="A21:A25" si="7">A20+TIME(0,F20,0)</f>
         <v>0.60416666666666663</v>
@@ -1397,7 +1425,7 @@
         <f t="shared" ref="B21:B25" si="8">A21+TIME(0,F21,0)</f>
         <v>0.61249999999999993</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="23" t="s">
         <v>102</v>
       </c>
       <c r="D21" s="10" t="s">
@@ -1410,7 +1438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <f t="shared" si="7"/>
         <v>0.61249999999999993</v>
@@ -1419,18 +1447,18 @@
         <f t="shared" si="8"/>
         <v>0.62083333333333324</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="16" t="s">
+      <c r="C22" s="23"/>
+      <c r="D22" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="22" t="s">
         <v>33</v>
       </c>
       <c r="F22" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <f t="shared" si="7"/>
         <v>0.62083333333333324</v>
@@ -1439,7 +1467,7 @@
         <f t="shared" si="8"/>
         <v>0.62916666666666654</v>
       </c>
-      <c r="C23" s="21"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="10" t="s">
         <v>34</v>
       </c>
@@ -1450,7 +1478,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <f t="shared" si="7"/>
         <v>0.62916666666666654</v>
@@ -1459,7 +1487,7 @@
         <f t="shared" si="8"/>
         <v>0.63749999999999984</v>
       </c>
-      <c r="C24" s="21"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="10" t="s">
         <v>36</v>
       </c>
@@ -1470,7 +1498,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <f t="shared" si="7"/>
         <v>0.63749999999999984</v>
@@ -1479,7 +1507,7 @@
         <f t="shared" si="8"/>
         <v>0.64583333333333315</v>
       </c>
-      <c r="C25" s="21"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="10" t="s">
         <v>94</v>
       </c>
@@ -1490,7 +1518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <f>A25+TIME(0,F25,0)</f>
         <v>0.64583333333333315</v>
@@ -1508,7 +1536,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <f>A26+TIME(0,F26,0)</f>
         <v>0.66666666666666652</v>
@@ -1544,33 +1572,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.1640625" style="1"/>
-    <col min="3" max="3" width="32.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="69.1640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="32.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1586,7 +1614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>0.375</v>
       </c>
@@ -1598,16 +1626,16 @@
         <v>100</v>
       </c>
       <c r="D3" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="F3" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <f t="shared" ref="A4:A20" si="0">A3+TIME(0,F3,0)</f>
         <v>0.40625</v>
@@ -1616,7 +1644,7 @@
         <f t="shared" ref="B4:B20" si="1">A4+TIME(0,F4,0)</f>
         <v>0.41458333333333336</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="25" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -1630,7 +1658,7 @@
       </c>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>0.41458333333333336</v>
@@ -1639,7 +1667,7 @@
         <f t="shared" si="1"/>
         <v>0.42291666666666672</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="10" t="s">
         <v>43</v>
       </c>
@@ -1651,7 +1679,7 @@
       </c>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <f t="shared" si="0"/>
         <v>0.42291666666666672</v>
@@ -1660,7 +1688,7 @@
         <f t="shared" si="1"/>
         <v>0.43125000000000008</v>
       </c>
-      <c r="C6" s="24"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="10" t="s">
         <v>45</v>
       </c>
@@ -1672,7 +1700,7 @@
       </c>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <f t="shared" si="0"/>
         <v>0.43125000000000008</v>
@@ -1681,7 +1709,7 @@
         <f t="shared" si="1"/>
         <v>0.43958333333333344</v>
       </c>
-      <c r="C7" s="24"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="10" t="s">
         <v>47</v>
       </c>
@@ -1693,7 +1721,7 @@
       </c>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>0.43958333333333344</v>
@@ -1702,7 +1730,7 @@
         <f t="shared" si="1"/>
         <v>0.4479166666666668</v>
       </c>
-      <c r="C8" s="24"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="10" t="s">
         <v>49</v>
       </c>
@@ -1714,7 +1742,7 @@
       </c>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>0.4479166666666668</v>
@@ -1723,7 +1751,7 @@
         <f t="shared" si="1"/>
         <v>0.45138888888888901</v>
       </c>
-      <c r="C9" s="24"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="10" t="s">
         <v>51</v>
       </c>
@@ -1735,7 +1763,7 @@
       </c>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>0.45138888888888901</v>
@@ -1744,7 +1772,7 @@
         <f t="shared" si="1"/>
         <v>0.45486111111111122</v>
       </c>
-      <c r="C10" s="24"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="10" t="s">
         <v>53</v>
       </c>
@@ -1756,7 +1784,7 @@
       </c>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <f t="shared" si="0"/>
         <v>0.45486111111111122</v>
@@ -1765,7 +1793,7 @@
         <f t="shared" si="1"/>
         <v>0.45833333333333343</v>
       </c>
-      <c r="C11" s="24"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="10" t="s">
         <v>55</v>
       </c>
@@ -1777,7 +1805,7 @@
       </c>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>0.45833333333333343</v>
@@ -1795,7 +1823,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <f t="shared" si="0"/>
         <v>0.47916666666666674</v>
@@ -1804,7 +1832,7 @@
         <f t="shared" si="1"/>
         <v>0.4875000000000001</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="25" t="s">
         <v>104</v>
       </c>
       <c r="D13" s="10" t="s">
@@ -1817,7 +1845,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <f t="shared" si="0"/>
         <v>0.4875000000000001</v>
@@ -1826,7 +1854,7 @@
         <f t="shared" si="1"/>
         <v>0.49583333333333346</v>
       </c>
-      <c r="C14" s="24"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="1" t="s">
         <v>59</v>
       </c>
@@ -1837,7 +1865,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <f t="shared" si="0"/>
         <v>0.49583333333333346</v>
@@ -1846,7 +1874,7 @@
         <f t="shared" si="1"/>
         <v>0.50416666666666676</v>
       </c>
-      <c r="C15" s="24"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="10" t="s">
         <v>61</v>
       </c>
@@ -1857,7 +1885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <f t="shared" si="0"/>
         <v>0.50416666666666676</v>
@@ -1866,7 +1894,7 @@
         <f t="shared" si="1"/>
         <v>0.51250000000000007</v>
       </c>
-      <c r="C16" s="24"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="10" t="s">
         <v>63</v>
       </c>
@@ -1877,7 +1905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <f t="shared" si="0"/>
         <v>0.51250000000000007</v>
@@ -1886,7 +1914,7 @@
         <f t="shared" si="1"/>
         <v>0.52083333333333337</v>
       </c>
-      <c r="C17" s="24"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="10" t="s">
         <v>65</v>
       </c>
@@ -1897,7 +1925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>0.52083333333333337</v>
@@ -1906,7 +1934,7 @@
         <f t="shared" si="1"/>
         <v>0.52430555555555558</v>
       </c>
-      <c r="C18" s="24"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="10" t="s">
         <v>67</v>
       </c>
@@ -1917,7 +1945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <f t="shared" si="0"/>
         <v>0.52430555555555558</v>
@@ -1926,7 +1954,7 @@
         <f t="shared" si="1"/>
         <v>0.52777777777777779</v>
       </c>
-      <c r="C19" s="24"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="10" t="s">
         <v>41</v>
       </c>
@@ -1937,7 +1965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <f t="shared" si="0"/>
         <v>0.52777777777777779</v>
@@ -1946,7 +1974,7 @@
         <f t="shared" si="1"/>
         <v>0.53125</v>
       </c>
-      <c r="C20" s="24"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="10" t="s">
         <v>70</v>
       </c>
@@ -1957,7 +1985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <f>A20+TIME(0,F20,0)</f>
         <v>0.53125</v>
@@ -1966,7 +1994,7 @@
         <f>A21+TIME(0,F21,0)</f>
         <v>0.53472222222222221</v>
       </c>
-      <c r="C21" s="24"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="10" t="s">
         <v>72</v>
       </c>
@@ -1977,264 +2005,296 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
         <f>A21+TIME(0,F21,0)</f>
         <v>0.53472222222222221</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="10">
         <f>A22+TIME(0,F22,0)</f>
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="10"/>
+      <c r="F22" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <f>A22+TIME(0,F22,0)</f>
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="B23" s="3">
+        <f>A23+TIME(0,F23,0)</f>
         <v>0.57986111111111105</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C23" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="4">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="10">
-        <f>A22+TIME(0,F22,0)</f>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <f>A23+TIME(0,F23,0)</f>
         <v>0.57986111111111105</v>
       </c>
-      <c r="B23" s="10">
-        <f>A23+TIME(0,F23,0)</f>
+      <c r="B24" s="10">
+        <f>A24+TIME(0,F24,0)</f>
         <v>0.5888888888888888</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C24" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="F23" s="1">
+      <c r="D24" s="10"/>
+      <c r="F24" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="10">
-        <f t="shared" ref="A24:A31" si="2">A23+TIME(0,F23,0)</f>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <f t="shared" ref="A25:A33" si="2">A24+TIME(0,F24,0)</f>
         <v>0.5888888888888888</v>
       </c>
-      <c r="B24" s="10">
-        <f t="shared" ref="B24:B31" si="3">A24+TIME(0,F24,0)</f>
+      <c r="B25" s="10">
+        <f t="shared" ref="B25:B33" si="3">A25+TIME(0,F25,0)</f>
         <v>0.5972222222222221</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="10" t="s">
+      <c r="C25" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F24" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="10">
+      <c r="F25" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
         <f t="shared" si="2"/>
         <v>0.5972222222222221</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B26" s="10">
         <f t="shared" si="3"/>
         <v>0.6055555555555554</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="10" t="s">
+      <c r="C26" s="26"/>
+      <c r="D26" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F25" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="10">
+      <c r="F26" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
         <f t="shared" si="2"/>
         <v>0.6055555555555554</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B27" s="10">
         <f t="shared" si="3"/>
         <v>0.61388888888888871</v>
       </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="10" t="s">
+      <c r="C27" s="26"/>
+      <c r="D27" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F26" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="10">
+      <c r="F27" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
         <f t="shared" si="2"/>
         <v>0.61388888888888871</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B28" s="10">
         <f t="shared" si="3"/>
         <v>0.62222222222222201</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="10" t="s">
+      <c r="C28" s="26"/>
+      <c r="D28" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="10">
+      <c r="F28" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
         <f t="shared" si="2"/>
         <v>0.62222222222222201</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B29" s="10">
         <f t="shared" si="3"/>
         <v>0.63055555555555531</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="10" t="s">
+      <c r="C29" s="26"/>
+      <c r="D29" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="10">
+      <c r="F29" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
         <f t="shared" si="2"/>
         <v>0.63055555555555531</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B30" s="10">
         <f t="shared" si="3"/>
         <v>0.63888888888888862</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="16" t="s">
+      <c r="C30" s="26"/>
+      <c r="D30" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E30" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="F29" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="10">
+      <c r="F30" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
         <f t="shared" si="2"/>
         <v>0.63888888888888862</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B31" s="10">
         <f t="shared" si="3"/>
         <v>0.64236111111111083</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="10" t="s">
+      <c r="C31" s="26"/>
+      <c r="D31" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F31" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="10">
+    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
         <f t="shared" si="2"/>
         <v>0.64236111111111083</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B32" s="10">
         <f t="shared" si="3"/>
         <v>0.64583333333333304</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="10" t="s">
+      <c r="C32" s="26"/>
+      <c r="D32" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F32" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
-        <f>A31+TIME(0,F31,0)</f>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <f t="shared" si="2"/>
         <v>0.64583333333333304</v>
       </c>
-      <c r="B32" s="3">
-        <f>A32+TIME(0,F32,0)</f>
+      <c r="B33" s="10">
+        <f t="shared" si="3"/>
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="C33" s="26"/>
+      <c r="D33" s="10"/>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <f>A33+TIME(0,F33,0)</f>
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="B34" s="3">
+        <f>A34+TIME(0,F34,0)</f>
         <v>0.66666666666666641</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C34" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="4">
+      <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="10">
-        <f>A32+TIME(0,F32,0)</f>
+    <row r="35" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <f>A34+TIME(0,F34,0)</f>
         <v>0.66666666666666641</v>
       </c>
-      <c r="B33" s="10">
-        <f>A33+TIME(0,F33,0)</f>
+      <c r="B35" s="10">
+        <f>A35+TIME(0,F35,0)</f>
         <v>0.69791666666666641</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C35" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="E33" s="17" t="s">
+      <c r="D35" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E35" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F35" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="10">
-        <f t="shared" ref="A34" si="4">A33+TIME(0,F33,0)</f>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <f t="shared" ref="A36" si="4">A35+TIME(0,F35,0)</f>
         <v>0.69791666666666641</v>
       </c>
-      <c r="B34" s="10">
-        <f t="shared" ref="B34" si="5">A34+TIME(0,F34,0)</f>
+      <c r="B36" s="10">
+        <f t="shared" ref="B36" si="5">A36+TIME(0,F36,0)</f>
         <v>0.70833333333333304</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C36" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="F34" s="1">
+      <c r="D36" s="10"/>
+      <c r="F36" s="1">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C4:C11"/>
-    <mergeCell ref="C24:C31"/>
+    <mergeCell ref="C25:C33"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C13:C21"/>
+    <mergeCell ref="C13:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="54" orientation="portrait" verticalDpi="597" r:id="rId1"/>

</xml_diff>